<commit_message>
Update use cases for new API
</commit_message>
<xml_diff>
--- a/final/UseCases.xlsx
+++ b/final/UseCases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Iniciar sessão" sheetId="1" state="visible" r:id="rId3"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="225">
   <si>
     <t xml:space="preserve">1. Dividir os fluxos 
     em sequências de transacções</t>
@@ -301,6 +301,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">e compatíveis com os dados presentes no sistema</t>
     </r>
@@ -373,35 +374,7 @@
     <t xml:space="preserve">(3)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[dados inválidos</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ou incompatíveis com dados já no sistema</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">] (passo 6):</t>
-    </r>
+    <t xml:space="preserve">[dados inválidos ou incompatíveis com dados já no sistema] (passo 6):</t>
   </si>
   <si>
     <t xml:space="preserve">6.1.</t>
@@ -447,9 +420,6 @@
   </si>
   <si>
     <t xml:space="preserve">Sistema informa que a operação de importação foi cancelada.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[dados inválidos ou incompatíveis com dados já no sistema] (passo 6):</t>
   </si>
   <si>
     <t xml:space="preserve">Definir preferências de uma UC</t>
@@ -600,7 +570,7 @@
     <t xml:space="preserve">Registar UCs de aluno</t>
   </si>
   <si>
-    <t xml:space="preserve">registarUCsDeAluno(numeroAluno: String, idUCs: Set(String)): void</t>
+    <t xml:space="preserve">registarUCsDeAluno(idCurso: String, numeroAluno: String, idUCs: Set(String)): void</t>
   </si>
   <si>
     <t xml:space="preserve">[aluno com o mesmo número já existe] (passo 4)</t>
@@ -645,25 +615,7 @@
     <t xml:space="preserve">Procurar sobreposicões</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">procurarSobreposicoes(idCurso: String): </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Collection(Sobreposicao)</t>
-    </r>
+    <t xml:space="preserve">procurarSobreposicoes(idCurso: String): Collection(Sobreposicao)</t>
   </si>
   <si>
     <t xml:space="preserve">Sistema informa ator de sucesso na geração de horários.</t>
@@ -726,35 +678,7 @@
     <t xml:space="preserve">Validar horário</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">validarHorario(numeroAluno: String, horario: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Map(String, Set(String))</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">): bool</t>
-    </r>
+    <t xml:space="preserve">validarHorario(numeroAluno: String, horario: Map(String, Set(String))): bool</t>
   </si>
   <si>
     <t xml:space="preserve">Sistema armazena horário modificado.</t>
@@ -763,35 +687,7 @@
     <t xml:space="preserve">Armazenar horário</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">armazenarHorario(idCurso: String, numeroAluno: String, horario: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Map(String, Set(String))</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">): void</t>
-    </r>
+    <t xml:space="preserve">armazenarHorario(idCurso: String, numeroAluno: String, horario: Map(String, Set(String))): void</t>
   </si>
   <si>
     <t xml:space="preserve">11.</t>
@@ -856,7 +752,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -922,25 +818,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1080,7 +958,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1552,7 +1430,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="54.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="5" min="5" style="1" width="5.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="6" min="6" style="1" width="53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="7" min="7" style="1" width="95.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="7" min="7" style="1" width="95.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="8" min="8" style="1" width="47.82"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="53.45"/>
@@ -1579,7 +1457,7 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="3"/>
@@ -1592,7 +1470,7 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
@@ -1623,7 +1501,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="3"/>
@@ -1635,7 +1513,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="3"/>
@@ -1665,7 +1543,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="11"/>
@@ -1677,7 +1555,7 @@
         <v>17</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="11"/>
@@ -1689,7 +1567,7 @@
         <v>21</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
@@ -1721,14 +1599,14 @@
         <v>70</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="G14" s="13" t="s">
         <v>196</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>197</v>
       </c>
       <c r="H14" s="14" t="s">
         <v>52</v>
@@ -1739,7 +1617,7 @@
         <v>83</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="11" t="s">
@@ -1752,17 +1630,17 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H16" s="11"/>
     </row>
@@ -1771,7 +1649,7 @@
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H17" s="11"/>
     </row>
@@ -1780,26 +1658,26 @@
         <v>89</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
     </row>
-    <row r="19" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="G19" s="13" t="s">
         <v>203</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>204</v>
       </c>
       <c r="H19" s="14" t="s">
         <v>52</v>
@@ -1807,17 +1685,17 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="G20" s="11" t="s">
         <v>206</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>207</v>
       </c>
       <c r="H20" s="14" t="s">
         <v>52</v>
@@ -1825,7 +1703,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>71</v>
@@ -1851,7 +1729,7 @@
         <v>26</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E23" s="11"/>
       <c r="G23" s="11"/>
@@ -1859,10 +1737,10 @@
     </row>
     <row r="24" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>211</v>
       </c>
       <c r="E24" s="12"/>
       <c r="G24" s="12"/>
@@ -1881,7 +1759,7 @@
         <v>99</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E26" s="11"/>
       <c r="G26" s="11"/>
@@ -1889,10 +1767,10 @@
     </row>
     <row r="27" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="11"/>
@@ -1940,7 +1818,7 @@
   </sheetPr>
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -1979,7 +1857,7 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="3"/>
@@ -1992,7 +1870,7 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
@@ -2028,7 +1906,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="3"/>
@@ -2040,7 +1918,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="3"/>
@@ -2070,7 +1948,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="11"/>
@@ -2102,7 +1980,7 @@
         <v>38</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="13" t="s">
@@ -2125,7 +2003,7 @@
       <c r="E13" s="12"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H13" s="13" t="s">
         <v>20</v>
@@ -2138,14 +2016,14 @@
         <v>80</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="G14" s="14" t="s">
         <v>222</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>223</v>
       </c>
       <c r="H14" s="14" t="s">
         <v>20</v>
@@ -2166,7 +2044,7 @@
         <v>26</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
@@ -2175,10 +2053,10 @@
     </row>
     <row r="17" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="11"/>
@@ -3161,7 +3039,7 @@
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
     </row>
-    <row r="15" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="1" t="s">
         <v>83</v>
       </c>
@@ -3291,7 +3169,7 @@
       <c r="G26" s="12"/>
       <c r="H26" s="11"/>
     </row>
-    <row r="27" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
@@ -3690,7 +3568,7 @@
         <v>103</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="E27" s="12"/>
       <c r="G27" s="11"/>
@@ -3782,7 +3660,7 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="3"/>
@@ -3795,7 +3673,7 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
@@ -3838,7 +3716,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="3"/>
@@ -3868,7 +3746,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="11"/>
@@ -3898,14 +3776,14 @@
         <v>21</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12" s="13" t="s">
         <v>126</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>127</v>
       </c>
       <c r="H12" s="14" t="s">
         <v>52</v>
@@ -3916,7 +3794,7 @@
         <v>23</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
@@ -3929,7 +3807,7 @@
         <v>70</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -3941,14 +3819,14 @@
         <v>83</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="G15" s="13" t="s">
         <v>131</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>132</v>
       </c>
       <c r="H15" s="14" t="s">
         <v>52</v>
@@ -3959,7 +3837,7 @@
         <v>87</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="11"/>
@@ -3971,7 +3849,7 @@
         <v>89</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
@@ -3980,17 +3858,17 @@
     </row>
     <row r="18" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>136</v>
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="G18" s="13" t="s">
         <v>137</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>138</v>
       </c>
       <c r="H18" s="14" t="s">
         <v>52</v>
@@ -3998,10 +3876,10 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="13"/>
@@ -4024,7 +3902,7 @@
         <v>26</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E21" s="11"/>
       <c r="G21" s="11"/>
@@ -4043,7 +3921,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>96</v>
@@ -4054,10 +3932,10 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="E24" s="11"/>
       <c r="G24" s="11"/>
@@ -4076,7 +3954,7 @@
         <v>99</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E26" s="11"/>
       <c r="G26" s="11"/>
@@ -4084,10 +3962,10 @@
     </row>
     <row r="27" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>146</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>147</v>
       </c>
       <c r="E27" s="11"/>
       <c r="G27" s="11"/>
@@ -4106,7 +3984,7 @@
         <v>103</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E29" s="12"/>
       <c r="G29" s="11"/>
@@ -4114,10 +3992,10 @@
     </row>
     <row r="30" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E30" s="11"/>
       <c r="G30" s="12"/>
@@ -4159,7 +4037,7 @@
   </sheetPr>
   <dimension ref="B1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B5" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B5" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -4198,7 +4076,7 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="3"/>
@@ -4211,7 +4089,7 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
@@ -4242,7 +4120,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="3"/>
@@ -4254,7 +4132,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="3"/>
@@ -4284,7 +4162,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="11"/>
@@ -4296,7 +4174,7 @@
         <v>17</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="11"/>
@@ -4308,7 +4186,7 @@
         <v>21</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
@@ -4321,14 +4199,14 @@
         <v>23</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="G13" s="13" t="s">
         <v>158</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>159</v>
       </c>
       <c r="H13" s="14" t="s">
         <v>52</v>
@@ -4339,7 +4217,7 @@
         <v>70</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="11" t="s">
@@ -4357,14 +4235,14 @@
         <v>83</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H15" s="14" t="s">
         <v>52</v>
@@ -4375,7 +4253,7 @@
         <v>87</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="11"/>
@@ -4387,7 +4265,7 @@
         <v>89</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
@@ -4396,17 +4274,17 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="G18" s="13" t="s">
         <v>166</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>167</v>
       </c>
       <c r="H18" s="14" t="s">
         <v>52</v>
@@ -4414,17 +4292,17 @@
     </row>
     <row r="19" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="G19" s="13" t="s">
         <v>169</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>170</v>
       </c>
       <c r="H19" s="14" t="s">
         <v>52</v>
@@ -4446,7 +4324,7 @@
         <v>26</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E21" s="11"/>
       <c r="G21" s="11"/>
@@ -4454,10 +4332,10 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>172</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>173</v>
       </c>
       <c r="E22" s="12"/>
       <c r="G22" s="12"/>
@@ -4542,7 +4420,7 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="3"/>
@@ -4555,7 +4433,7 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
@@ -4586,7 +4464,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="3"/>
@@ -4598,7 +4476,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="3"/>
@@ -4628,7 +4506,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="11"/>
@@ -4658,14 +4536,14 @@
         <v>38</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H12" s="14" t="s">
         <v>52</v>
@@ -4676,7 +4554,7 @@
         <v>80</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="13"/>
@@ -4685,19 +4563,19 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="5" t="s">
         <v>70</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="G14" s="13" t="s">
         <v>183</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>184</v>
       </c>
       <c r="H14" s="14" t="s">
         <v>52</v>
@@ -4709,7 +4587,7 @@
         <v>83</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
@@ -4730,7 +4608,7 @@
         <v>26</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="11"/>
@@ -4742,7 +4620,7 @@
         <v>93</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="13"/>
@@ -4762,7 +4640,7 @@
       <c r="D20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="0"/>
+      <c r="D21" s="21"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="9"/>

</xml_diff>